<commit_message>
Working for large text files (40 x 40) image output
</commit_message>
<xml_diff>
--- a/mapping_image/pixel size calcs.xlsx
+++ b/mapping_image/pixel size calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aeon 3200\PycharmProjects\TextWeaver\mapping_image\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FA2EF29-352A-4BAC-A86A-D4D8DDADD550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CF17EE-6B49-43D6-93C6-290C40971F8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30765" yWindow="480" windowWidth="23235" windowHeight="16875" xr2:uid="{94DB29C5-18FE-4778-BE45-4A7F185D97C3}"/>
+    <workbookView xWindow="28800" yWindow="525" windowWidth="23235" windowHeight="16875" xr2:uid="{94DB29C5-18FE-4778-BE45-4A7F185D97C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>width inches</t>
   </si>
@@ -42,6 +42,36 @@
   </si>
   <si>
     <t>total pixels</t>
+  </si>
+  <si>
+    <t>Max size</t>
+  </si>
+  <si>
+    <t>works</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total pixels </t>
+  </si>
+  <si>
+    <t>try</t>
+  </si>
+  <si>
+    <t>wide</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>15 inch wide at 300 ppi</t>
+  </si>
+  <si>
+    <t>44 inch wide at 300 ppi</t>
+  </si>
+  <si>
+    <t>44 inch wide at 300 ppi (26 inches high</t>
   </si>
 </sst>
 </file>
@@ -393,15 +423,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D2B8B5-837B-4911-B1DD-B60B3D96200B}">
-  <dimension ref="A3:C14"/>
+  <dimension ref="A3:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,6 +554,89 @@
         <v>1224</v>
       </c>
     </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>20000</v>
+      </c>
+      <c r="C20">
+        <v>4500</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <f>+ B20*C20</f>
+        <v>90000000</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <f>+F21/C21</f>
+        <v>6818.181818181818</v>
+      </c>
+      <c r="C21">
+        <v>13200</v>
+      </c>
+      <c r="F21">
+        <f>+$F20</f>
+        <v>90000000</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>13200</v>
+      </c>
+      <c r="C22">
+        <v>13200</v>
+      </c>
+      <c r="H22" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22">
+        <f>13200/300</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>+ 40 * 300</f>
+        <v>12000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>